<commit_message>
Archivos del guión 12 de 6
Archivos actualizados con modificaciones del autor y editor, listo para
corrección de estilo
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion11/SolicitudGrafica_CN_06_11_REC260.xlsx
+++ b/fuentes/contenidos/grado06/guion11/SolicitudGrafica_CN_06_11_REC260.xlsx
@@ -1745,15 +1745,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1916205</xdr:colOff>
+      <xdr:colOff>2008910</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>302559</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>4471147</xdr:colOff>
+      <xdr:colOff>4523102</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2334823</xdr:rowOff>
+      <xdr:rowOff>2302409</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1777,8 +1777,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="18265587" y="2297206"/>
-          <a:ext cx="2554942" cy="2032264"/>
+          <a:off x="18339955" y="2276832"/>
+          <a:ext cx="2514192" cy="1999850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2913,8 +2913,8 @@
   <dimension ref="A1:P95"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>

</xml_diff>